<commit_message>
Edit data file column names
</commit_message>
<xml_diff>
--- a/data/Battery Parameters.xlsx
+++ b/data/Battery Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://auroraer-my.sharepoint.com/personal/ulysse_schnyder_auroraer_com/Documents/Admin/SEM technical challenge/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/basharanwar/Research/Aurora/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{B22F2BA3-B3F2-4578-BE00-ED228F88B26E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{767B9C97-2F87-46D6-9514-585F7ED5A2C2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E3245F-EB2D-2642-B8E4-D7B0BD2C45DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18BF1BF6-01D1-4441-B39A-1BFD0393B104}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{18BF1BF6-01D1-4441-B39A-1BFD0393B104}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>MWh</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Maximum battery lifetime in battery cycles equivalent - one cycle is defined as charging up to max storage volume and then discharging all stored energy. This does not have to be done in one go - e.g. charging up to 75%, discharging to 0%, then charging up to 25% and discharging to 0% still counts as one cycle.</t>
+  </si>
+  <si>
+    <t>Parameters</t>
   </si>
 </sst>
 </file>
@@ -134,7 +137,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -164,10 +167,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -186,7 +188,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -474,7 +476,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -485,16 +487,19 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="24.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
@@ -505,7 +510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -519,7 +524,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -533,7 +538,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -547,7 +552,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -561,7 +566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -575,7 +580,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -589,7 +594,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -603,7 +608,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -617,11 +622,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>500000</v>
       </c>
       <c r="C10" t="s">
@@ -631,7 +636,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>5</v>
       </c>

</xml_diff>